<commit_message>
Añadidos precios del día 26 al script inicial
</commit_message>
<xml_diff>
--- a/SeguimientoCartera/sql/01_seguimiento_cartera.xlsx
+++ b/SeguimientoCartera/sql/01_seguimiento_cartera.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_JSM\SeguimientoCartera\03_Fuentes\markets_data\SeguimientoCartera\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_JSM\SeguimientoCartera\03_Fuentes\markets_data\SeguimientoCartera\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER_MOVIMIENTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="160">
   <si>
     <t>iShares UltraHQ EurGovtBdIdx(IE)InstAcc€</t>
   </si>
@@ -888,7 +888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4418,11 +4418,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F28"/>
+  <dimension ref="B1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4461,10 +4459,10 @@
         <v>29</v>
       </c>
       <c r="D3" s="2">
-        <v>144.43</v>
+        <v>144.47999999999999</v>
       </c>
       <c r="E3" s="3">
-        <v>44221</v>
+        <v>44222</v>
       </c>
       <c r="F3" s="3"/>
     </row>
@@ -4784,29 +4782,27 @@
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>107</v>
+        <v>157</v>
       </c>
       <c r="D25" s="2">
-        <v>12.38</v>
+        <v>13.75</v>
       </c>
       <c r="E25" s="3">
-        <v>44221</v>
+        <v>44222</v>
       </c>
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D26" s="2">
-        <v>13.29</v>
+        <v>12.38</v>
       </c>
       <c r="E26" s="3">
         <v>44221</v>
@@ -4815,13 +4811,13 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D27" s="2">
-        <v>207.4</v>
+        <v>13.27</v>
       </c>
       <c r="E27" s="3">
         <v>44222</v>
@@ -4830,18 +4826,33 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D28" s="2">
-        <v>6.53</v>
+        <v>207.4</v>
       </c>
       <c r="E28" s="3">
         <v>44222</v>
       </c>
       <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="2">
+        <v>6.53</v>
+      </c>
+      <c r="E29" s="3">
+        <v>44222</v>
+      </c>
+      <c r="F29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>